<commit_message>
start question 3, 4, and 5
</commit_message>
<xml_diff>
--- a/assignment_3/assignment_3.xlsx
+++ b/assignment_3/assignment_3.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\University\3B\MSCI_261\assignment_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7BA6CA-1588-4573-9AB6-27612DE62618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC737C6-1ABA-4601-9AD6-D00161BB4744}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="2424" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{7198FCC0-B348-45CC-9ADF-D17D806C4162}"/>
+    <workbookView xWindow="-4224" yWindow="3324" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="4" xr2:uid="{7198FCC0-B348-45CC-9ADF-D17D806C4162}"/>
   </bookViews>
   <sheets>
     <sheet name="Question 1" sheetId="1" r:id="rId1"/>
     <sheet name="Question 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Question 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Question 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Question 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="53">
   <si>
     <t>Year</t>
   </si>
@@ -111,6 +114,111 @@
   <si>
     <t>EAC (defender) &gt; EAC (challenger) --&gt; YES</t>
   </si>
+  <si>
+    <t>Initial Cost ($)</t>
+  </si>
+  <si>
+    <t>M&amp;O ($)</t>
+  </si>
+  <si>
+    <t>Salvage Value ($)</t>
+  </si>
+  <si>
+    <t>Period (years)</t>
+  </si>
+  <si>
+    <t>Depreciation Rate</t>
+  </si>
+  <si>
+    <t>PV of M&amp;O</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Period (Years)</t>
+  </si>
+  <si>
+    <t>O &amp; M ($)</t>
+  </si>
+  <si>
+    <t>Depreciation ($)</t>
+  </si>
+  <si>
+    <t>Purchasing Price</t>
+  </si>
+  <si>
+    <t>Annual Interest Rate</t>
+  </si>
+  <si>
+    <t>PV of O &amp; M</t>
+  </si>
+  <si>
+    <t>Initial Cost</t>
+  </si>
+  <si>
+    <t>Initial cost</t>
+  </si>
+  <si>
+    <t>Useful life (years)</t>
+  </si>
+  <si>
+    <t>Annual savings in costs on the 1st year</t>
+  </si>
+  <si>
+    <t>Increase amount in annual savings starting from year 2</t>
+  </si>
+  <si>
+    <t>Additional annual operating cost</t>
+  </si>
+  <si>
+    <t>Salvage value</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>CTF</t>
+  </si>
+  <si>
+    <t>Tax Rate</t>
+  </si>
+  <si>
+    <t>CCA</t>
+  </si>
+  <si>
+    <t>CSF</t>
+  </si>
+  <si>
+    <t>Salvage Value</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Increase Amount in Annual Savings</t>
+  </si>
+  <si>
+    <t>Additional Annual Operating Cost</t>
+  </si>
+  <si>
+    <t>Annual Savings in Costs</t>
+  </si>
+  <si>
+    <t>(P/A, 12%, 5)</t>
+  </si>
+  <si>
+    <t>(A/G, 12%, 5)</t>
+  </si>
+  <si>
+    <t>(P/F, 12%, 5)</t>
+  </si>
+  <si>
+    <t>Selection</t>
+  </si>
 </sst>
 </file>
 
@@ -153,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -174,6 +282,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1625,6 +1745,1246 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>EAC of Defender</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>EAC (capital)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Question 3'!$A$12:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Question 3'!$B$12:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12035.186436852615</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10309.152258134469</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8970.283215892412</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7922.4638212613017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7094.9370198686311</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B581-448A-9888-99811EB82B8B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>EAC (op. cost)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Question 3'!$A$12:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Question 3'!$C$12:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74761.904761904763</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79365.55891238671</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83811.678517560853</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88101.259602627295</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B581-448A-9888-99811EB82B8B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>EAC (total)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Question 3'!$A$12:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Question 3'!$D$12:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82035.186436852615</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85071.057020039239</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88335.842128279124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91734.142338822159</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95196.196622495932</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B581-448A-9888-99811EB82B8B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="557372160"/>
+        <c:axId val="557370520"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="557372160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Time (Years)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="557370520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="557370520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Amount ($)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="557372160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>EAC of Challenger</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>EAC (capital)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Question 3'!$E$12:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70439.367138168425</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59026.645207766669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50456.81746227145</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43943.475257442777</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38931.647311264336</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E41B-432D-A388-D9123904FD60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>EAC (op. cost)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Question 3'!$F$12:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30000.000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30952.380952380954</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32477.341389728099</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34960.137901314367</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37423.629424579442</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E41B-432D-A388-D9123904FD60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>EAC (total)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Question 3'!$G$12:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100439.36713816843</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89979.026160147623</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82934.158851999557</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78903.613158757144</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76355.27673584377</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E41B-432D-A388-D9123904FD60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="433312336"/>
+        <c:axId val="433312664"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="433312336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Time (Years)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433312664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="433312664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Amount ($)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433312336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1705,6 +3065,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2209,6 +3649,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2768,6 +5214,83 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8038A6D-D993-4A41-A22A-C416A8BF8EA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>767040</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4E114C7-E1FD-4EE4-A77A-CA4AF7308F9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>792480</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>538440</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F83FC4F0-B1D9-4974-BAE5-63C947D141AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3087,8 +5610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F91415-D79B-4B44-B03D-E3FF2293C478}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3104,23 +5627,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="E1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -3133,7 +5656,7 @@
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -3240,16 +5763,16 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="6" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -3494,8 +6017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85784B83-B326-498E-8866-A2FB17981F09}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3510,23 +6033,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="G1" s="6" t="s">
+      <c r="E1" s="9"/>
+      <c r="G1" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
@@ -3539,7 +6062,7 @@
       <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -3630,22 +6153,22 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
@@ -3757,10 +6280,11 @@
         <v>12229.607250755282</v>
       </c>
       <c r="F14" s="5">
-        <v>1000</v>
+        <f xml:space="preserve"> E6 * (1 / ((1 + G3)^A14)) * (G3 * ((1 + G3)^A14) / ((1 + G3)^A14 - 1))</f>
+        <v>302.11480362537731</v>
       </c>
       <c r="G14" s="5">
-        <v>13229.607250755282</v>
+        <v>12531.72205438066</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -3807,7 +6331,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -3831,4 +6355,995 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6FAF7F-F4D3-419A-9F42-945B31CF036A}">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>30000</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5">
+        <v>30000</v>
+      </c>
+      <c r="E3" s="5">
+        <v>160000</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5">
+        <v>160000</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5">
+        <v>70000</v>
+      </c>
+      <c r="D4" s="5" cm="1">
+        <f t="array" ref="D4:D7" xml:space="preserve"> D3 * (1 - A21)^A4:A7</f>
+        <v>20964.813563147378</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5">
+        <v>30000</v>
+      </c>
+      <c r="G4" s="5" cm="1">
+        <f t="array" ref="G4:G7" xml:space="preserve"> E3 * (1 - B21)^A4:A7</f>
+        <v>105560.63286183153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5">
+        <v>80000</v>
+      </c>
+      <c r="D5" s="5">
+        <v>14650.780257917606</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
+        <v>32000</v>
+      </c>
+      <c r="G5" s="5">
+        <v>69644.045063689919</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5">
+        <v>90000</v>
+      </c>
+      <c r="D6" s="5">
+        <v>10238.362555396096</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
+        <v>36000</v>
+      </c>
+      <c r="G6" s="5">
+        <v>45947.934199881398</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5">
+        <v>100000</v>
+      </c>
+      <c r="D7" s="5">
+        <v>7154.8454055262764</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5">
+        <v>44000</v>
+      </c>
+      <c r="G7" s="5">
+        <v>30314.331330207951</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5">
+        <v>110000</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5000</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
+        <v>50000</v>
+      </c>
+      <c r="G8" s="5">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
+      <c r="B11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>0</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" cm="1">
+        <f t="array" ref="B13:B17" xml:space="preserve"> (D3 - D4:D8) * ((I3 * (1 + I3)^A13:A17) / ((1 + I3)^A13:A17 - 1)) + D4:D8 * I3</f>
+        <v>12035.186436852615</v>
+      </c>
+      <c r="C13" s="5">
+        <f xml:space="preserve"> -PMT($I$3, A13, SUM($E$22:E22))</f>
+        <v>70000</v>
+      </c>
+      <c r="D13" s="5">
+        <f xml:space="preserve"> B13 + C13</f>
+        <v>82035.186436852615</v>
+      </c>
+      <c r="E13" s="5" cm="1">
+        <f t="array" ref="E13:E17" xml:space="preserve"> (G3 - G4:G8) * ((I3 * (1 + I3)^A13:A17) / ((1 + I3)^A13:A17 - 1)) + G4:G8 * I3</f>
+        <v>70439.367138168425</v>
+      </c>
+      <c r="F13" s="5">
+        <f xml:space="preserve"> -PMT($I$3, A13, SUM($F$22:F22))</f>
+        <v>30000.000000000007</v>
+      </c>
+      <c r="G13" s="5">
+        <f xml:space="preserve"> E13 + F13</f>
+        <v>100439.36713816843</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5">
+        <v>10309.152258134469</v>
+      </c>
+      <c r="C14" s="5">
+        <f xml:space="preserve"> -PMT($I$3, A14, SUM($E$22:E23))</f>
+        <v>74761.904761904763</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" ref="D14:D17" si="0" xml:space="preserve"> B14 + C14</f>
+        <v>85071.057020039239</v>
+      </c>
+      <c r="E14" s="5">
+        <v>59026.645207766669</v>
+      </c>
+      <c r="F14" s="5">
+        <f xml:space="preserve"> -PMT($I$3, A14, SUM($F$22:F23))</f>
+        <v>30952.380952380954</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" ref="G14:G17" si="1" xml:space="preserve"> E14 + F14</f>
+        <v>89979.026160147623</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5">
+        <v>8970.283215892412</v>
+      </c>
+      <c r="C15" s="5">
+        <f xml:space="preserve"> -PMT($I$3, A15, SUM($E$22:E24))</f>
+        <v>79365.55891238671</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>88335.842128279124</v>
+      </c>
+      <c r="E15" s="5">
+        <v>50456.81746227145</v>
+      </c>
+      <c r="F15" s="5">
+        <f xml:space="preserve"> -PMT($I$3, A15, SUM($F$22:F24))</f>
+        <v>32477.341389728099</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="1"/>
+        <v>82934.158851999557</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>4</v>
+      </c>
+      <c r="B16" s="5">
+        <v>7922.4638212613017</v>
+      </c>
+      <c r="C16" s="5">
+        <f xml:space="preserve"> -PMT($I$3, A16, SUM($E$22:E25))</f>
+        <v>83811.678517560853</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>91734.142338822159</v>
+      </c>
+      <c r="E16" s="5">
+        <v>43943.475257442777</v>
+      </c>
+      <c r="F16" s="5">
+        <f xml:space="preserve"> -PMT($I$3, A16, SUM($F$22:F25))</f>
+        <v>34960.137901314367</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="1"/>
+        <v>78903.613158757144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5">
+        <v>7094.9370198686311</v>
+      </c>
+      <c r="C17" s="5">
+        <f xml:space="preserve"> -PMT($I$3, A17, SUM($E$22:E26))</f>
+        <v>88101.259602627295</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>95196.196622495932</v>
+      </c>
+      <c r="E17" s="5">
+        <v>38931.647311264336</v>
+      </c>
+      <c r="F17" s="5">
+        <f xml:space="preserve"> -PMT($I$3, A17, SUM($F$22:F26))</f>
+        <v>37423.629424579442</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="1"/>
+        <v>76355.27673584377</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="D19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <f xml:space="preserve"> 1 - (D8 / D3)^(1 / A8)</f>
+        <v>0.30117288122842079</v>
+      </c>
+      <c r="B21" s="7">
+        <f xml:space="preserve"> 1 - (G8 / E3)^(1 / A8)</f>
+        <v>0.3402460446135529</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5" cm="1">
+        <f t="array" ref="E22:E26" xml:space="preserve"> C4:C8 / (1 + I3)^A4:A8</f>
+        <v>63636.363636363632</v>
+      </c>
+      <c r="F22" s="5" cm="1">
+        <f t="array" ref="F22:F26" xml:space="preserve"> F4:F8 / (1 + I3)^A4:A8</f>
+        <v>27272.727272727272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D23" s="7">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5">
+        <v>66115.702479338826</v>
+      </c>
+      <c r="F23" s="5">
+        <v>26446.280991735533</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D24" s="7">
+        <v>3</v>
+      </c>
+      <c r="E24" s="5">
+        <v>67618.332081141984</v>
+      </c>
+      <c r="F24" s="5">
+        <v>27047.332832456792</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D25" s="7">
+        <v>4</v>
+      </c>
+      <c r="E25" s="5">
+        <v>68301.345536507055</v>
+      </c>
+      <c r="F25" s="5">
+        <v>30052.592036063103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D26" s="7">
+        <v>5</v>
+      </c>
+      <c r="E26" s="5">
+        <v>68301.34553650704</v>
+      </c>
+      <c r="F26" s="5">
+        <v>31046.066152957748</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE5D73E-702F-49DA-8EF8-7F5EE05E45F2}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="7"/>
+    <col min="8" max="8" width="20.33203125" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>100</v>
+      </c>
+      <c r="C2" s="7">
+        <v>210</v>
+      </c>
+      <c r="D2" s="7">
+        <v>590</v>
+      </c>
+      <c r="F2" s="7">
+        <v>800</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>180</v>
+      </c>
+      <c r="C3" s="7">
+        <v>140</v>
+      </c>
+      <c r="D3" s="7">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7">
+        <v>270</v>
+      </c>
+      <c r="C4" s="7">
+        <v>260</v>
+      </c>
+      <c r="D4" s="7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" cm="1">
+        <f t="array" ref="B7:B9" xml:space="preserve"> (F2- D2:D4) * ((H2 * (1 + H2)^A7:A9) / ((1 + H2)^A7:A9 - 1)) + D2:D4 * H2</f>
+        <v>289.99999999999983</v>
+      </c>
+      <c r="C7" s="5">
+        <f xml:space="preserve"> -PMT($H$2, A7, SUM($B$12:B12))</f>
+        <v>100.00000000000001</v>
+      </c>
+      <c r="D7" s="5">
+        <f xml:space="preserve"> B7 + C7</f>
+        <v>389.99999999999983</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5">
+        <v>246.66666666666654</v>
+      </c>
+      <c r="C8" s="5">
+        <f xml:space="preserve"> -PMT($H$2, A8, SUM($B$12:B13))</f>
+        <v>138.0952380952381</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" ref="D8:D9" si="0" xml:space="preserve"> B8 + C8</f>
+        <v>384.76190476190465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5">
+        <v>264.29003021148014</v>
+      </c>
+      <c r="C9" s="5">
+        <f xml:space="preserve"> -PMT($H$2, A9, SUM($B$12:B14))</f>
+        <v>177.94561933534743</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>442.23564954682757</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5" cm="1">
+        <f t="array" ref="B12:B14" xml:space="preserve"> B2:B4 / (1 + H2)^A12:A14</f>
+        <v>90.909090909090907</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5">
+        <v>148.76033057851237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5">
+        <v>202.85499624342594</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="7">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDAD269F-E081-471B-AD6D-68AB2FF7A0AE}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.21875" style="7" customWidth="1"/>
+    <col min="2" max="3" width="9.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="7"/>
+    <col min="5" max="5" width="13.44140625" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="7">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="7">
+        <v>60000</v>
+      </c>
+      <c r="C3" s="7">
+        <v>76000</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="7">
+        <v>25000</v>
+      </c>
+      <c r="C4" s="7">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="7">
+        <v>5000</v>
+      </c>
+      <c r="C5" s="7">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="7">
+        <v>6000</v>
+      </c>
+      <c r="C6" s="7">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="4">
+        <f xml:space="preserve"> 1 - (F2 * F3 / (F1 + F3)) * ((1 + F1 / 2) / (1 + F1))</f>
+        <v>0.7633928571428571</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="7">
+        <v>3.6048</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="7">
+        <f xml:space="preserve"> 1 - F2 * F3 / (F1 + F3)</f>
+        <v>0.75</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1.7746</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.56742999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="11">
+        <f xml:space="preserve"> -B3 * B9</f>
+        <v>-45803.571428571428</v>
+      </c>
+      <c r="C13" s="11">
+        <f xml:space="preserve"> -C3 * B9</f>
+        <v>-58017.857142857138</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="11">
+        <f xml:space="preserve"> B4 * F9 * (1 - F2)</f>
+        <v>54072</v>
+      </c>
+      <c r="C14" s="11">
+        <f xml:space="preserve"> C4 * F9 * (1 - F2)</f>
+        <v>64886.399999999994</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="11">
+        <f xml:space="preserve"> B5 * F10 * F9 * (1 - F2)</f>
+        <v>19191.234239999998</v>
+      </c>
+      <c r="C15" s="11">
+        <f xml:space="preserve"> C5 * F10 * F9 * (1 - F2)</f>
+        <v>23029.481088</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="5">
+        <f xml:space="preserve"> -B6 * F9 * (1 - F2)</f>
+        <v>-12977.279999999999</v>
+      </c>
+      <c r="C16" s="5">
+        <f xml:space="preserve"> -C6 * F9 * (1 - F2)</f>
+        <v>-17303.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="5">
+        <f xml:space="preserve"> B7 * B10 * F11</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <f xml:space="preserve"> C7 * B10 * F11</f>
+        <v>2127.8625000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="5">
+        <f xml:space="preserve"> B13 + B14 + B15 + B16 + B17</f>
+        <v>14482.382811428572</v>
+      </c>
+      <c r="C18" s="5">
+        <f xml:space="preserve"> C13 + C14 + C15 + C16 + C17</f>
+        <v>14722.846445142855</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>